<commit_message>
changed the way effect sizes are estimated
</commit_message>
<xml_diff>
--- a/primary_outcomesRCT.xlsx
+++ b/primary_outcomesRCT.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -77,145 +77,145 @@
     <t xml:space="preserve">UPDRS_III_item20_22__clozapine_baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__clozapine_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__placebo_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__placebo_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
+    <t xml:space="preserve">UPDRS_III_items20_21__clozapine_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__placebo_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__placebo_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
   </si>
   <si>
     <t xml:space="preserve">Cattaneo et al. 2016</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__safinamide_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__placebo_mean-difference</t>
+    <t xml:space="preserve">UPDRS_III_items20_21__safinamide_mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__placebo_mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Craig et al. 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__nmt_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__nmt_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__music-relaxation_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__music-relaxation_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de Faria et al. 2020</t>
   </si>
   <si>
     <t xml:space="preserve">17</t>
   </si>
   <si>
-    <t xml:space="preserve">Craig et al. 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__nmt_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__nmt_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__music-relaxation_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__music-relaxation_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de Faria et al. 2020</t>
+    <t xml:space="preserve">Eberhardt et al. 1990</t>
   </si>
   <si>
     <t xml:space="preserve">19</t>
   </si>
   <si>
-    <t xml:space="preserve">Eberhardt et al. 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
     <t xml:space="preserve">Elmer (2013)</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__rasagiline_adjusted-mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__placebo_adjusted-mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
+    <t xml:space="preserve">UPDRS_item16_20_21__rasagiline_adjusted-mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_item16_20_21__placebo_adjusted-mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
   </si>
   <si>
     <t xml:space="preserve">Parkinson Study Group (1999)</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__clozapine_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
+    <t xml:space="preserve">UPDRS_III_items20_21__clozapine_mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
   </si>
   <si>
     <t xml:space="preserve">Goetz et al. 2000</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__placebo_percentual-change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31</t>
+    <t xml:space="preserve">UPDRS_III_items20_21__placebo_percentual-change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
   </si>
   <si>
     <t xml:space="preserve">Hattori et al. 2018</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__rasagiline_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__rasagiline_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32</t>
+    <t xml:space="preserve">UPDRS_III_items20_21__rasagiline_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__rasagiline_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
   </si>
   <si>
     <t xml:space="preserve">Heinonen et al. 1989</t>
   </si>
   <si>
-    <t xml:space="preserve">37</t>
+    <t xml:space="preserve">35</t>
   </si>
   <si>
     <t xml:space="preserve">Jankovic et al. 2014</t>
   </si>
   <si>
+    <t xml:space="preserve">39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kadkhodaie et al. 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaut et al. 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__wbv_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__wbv_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__control_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__control_follow-up</t>
+  </si>
+  <si>
     <t xml:space="preserve">41</t>
   </si>
   <si>
-    <t xml:space="preserve">Kadkhodaie et al. 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaut et al. 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__wbv_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__wbv_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__control_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__control_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43</t>
-  </si>
-  <si>
     <t xml:space="preserve">King et al. 2009</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__vibration_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__vibration_follow-up</t>
+    <t xml:space="preserve">UPDRS_III_items20_21__vibration_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__vibration_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">45</t>
@@ -224,22 +224,22 @@
     <t xml:space="preserve">Kulisevsky et al. 2002</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__theophylline_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__theophylline_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__placebo-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__placebo-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__theophylline-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__theophylline-levodopa_follow-up</t>
+    <t xml:space="preserve">UPDRS_III_items20_21__theophylline_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__theophylline_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__placebo-levodopa_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__placebo-levodopa_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__theophylline-levodopa_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__theophylline-levodopa_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">46</t>
@@ -254,6 +254,12 @@
     <t xml:space="preserve">Lew (2013)</t>
   </si>
   <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__rasagiline_adjusted-mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__placebo_adjusted-mean-difference</t>
+  </si>
+  <si>
     <t xml:space="preserve">49</t>
   </si>
   <si>
@@ -266,22 +272,22 @@
     <t xml:space="preserve">Li et al. 2018</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__WG_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__WG_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__TAG_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__TAG_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__SAG_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__SAG_follow-up</t>
+    <t xml:space="preserve">UPDRS_III_items20_21__WG_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__WG_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__TAG_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__TAG_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__SAG_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__SAG_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">51</t>
@@ -308,322 +314,289 @@
     <t xml:space="preserve">Malsch et al. 2001</t>
   </si>
   <si>
-    <t xml:space="preserve">57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mannen et al. 1991</t>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mizuno et al. 1995.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pergolide_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pergolide_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine-levodopa_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine-levodopa_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pergolide-levodopa_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pergolide-levodopa_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">61</t>
   </si>
   <si>
-    <t xml:space="preserve">Mittal et al. 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS III section 20 change (rest tremor) median</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS III section 20 change (rest tremor) range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mizuno et al. 1995.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__bromocriptine_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__bromocriptine_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__pergolide_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__pergolide_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__bromocriptine-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__bromocriptine-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__pergolide-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__pergolide-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
     <t xml:space="preserve">Moeller et al. 2005</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__pramipexole_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__pramipexole_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__placebo_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__placebo_follow-up</t>
+    <t xml:space="preserve">UPDRS_items16_20_21__pramipexole_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__pramipexole_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__placebo_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__placebo_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montastruc et al. 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__piribedil50_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__piribedil50_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__piribedil100_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__piribedil100_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">66</t>
   </si>
   <si>
-    <t xml:space="preserve">Montastruc et al. 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__piribedil50_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__piribedil50_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__piribedil100_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__piribedil100_follow-up</t>
+    <t xml:space="preserve">Navan et al. 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navan et al. 2003.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nigro et al. 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__apomorphine_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__apomorphine_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__placebo_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__placebo_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nomoto et al. 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items16_20_21__rotigotine_mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items16_20_21__placebo_mean-difference</t>
   </si>
   <si>
     <t xml:space="preserve">70</t>
   </si>
   <si>
-    <t xml:space="preserve">Navan et al. 2003</t>
+    <t xml:space="preserve">Nomoto et al. 2018.1</t>
   </si>
   <si>
     <t xml:space="preserve">71</t>
   </si>
   <si>
-    <t xml:space="preserve">Navan et al. 2003.1</t>
+    <t xml:space="preserve">Nutt et al. 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olanow et al. 1987</t>
   </si>
   <si>
     <t xml:space="preserve">73</t>
   </si>
   <si>
-    <t xml:space="preserve">Nomoto et al. 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items16_20_21__rotigotine_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items16_20_21__placebo_mean-difference</t>
+    <t xml:space="preserve">Olson et al. 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__gabapentin_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__gabapentin_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">74</t>
   </si>
   <si>
-    <t xml:space="preserve">Nomoto et al. 2018.1</t>
+    <t xml:space="preserve">Parkinson Study Group (2007)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pramipexole_mean-difference</t>
   </si>
   <si>
     <t xml:space="preserve">75</t>
   </si>
   <si>
-    <t xml:space="preserve">Nutt et al. 2007</t>
+    <t xml:space="preserve">Petramfar et al. 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__licorice_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__licorice_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">76</t>
   </si>
   <si>
-    <t xml:space="preserve">Olanow et al. 1987</t>
+    <t xml:space="preserve">Pogarell et al. 2002</t>
   </si>
   <si>
     <t xml:space="preserve">78</t>
   </si>
   <si>
-    <t xml:space="preserve">Olson et al. 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__gabapentin_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__gabapentin_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parkinson Study Group (2007)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__pramipexole_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__pramipexole_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petramfar et al. 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__licorice_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item16_20_21__licorice_follow-up</t>
+    <t xml:space="preserve">Przuntek et al. 2002</t>
   </si>
   <si>
     <t xml:space="preserve">81</t>
   </si>
   <si>
-    <t xml:space="preserve">Pogarell et al. 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postuma et al. 2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__caffeine_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item21__caffeine_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Przuntek et al. 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rascol et al. 1988</t>
   </si>
   <si>
+    <t xml:space="preserve">96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huebsch et al. 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__qigong_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__qigong_follow-up</t>
+  </si>
+  <si>
     <t xml:space="preserve">97</t>
   </si>
   <si>
-    <t xml:space="preserve">Tortolero et al. 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__piribedil-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__piribedil-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__placebo-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__placebo-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item21__piribedil-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item21__piribedil-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item21__placebo-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item21__placebo-levodopa_follow-up</t>
+    <t xml:space="preserve">Schneider et al. 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__GM1_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__GM1_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schrag et al. 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__ropinirole_mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schrag et al. 2002.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine_mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schrag et al. 2002.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__levodopa_mean-difference</t>
   </si>
   <si>
     <t xml:space="preserve">102</t>
   </si>
   <si>
-    <t xml:space="preserve">Schneider et al. 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__GM1_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__GM1_follow-up</t>
+    <t xml:space="preserve">Sivertsen et al. 1989</t>
   </si>
   <si>
     <t xml:space="preserve">104</t>
   </si>
   <si>
-    <t xml:space="preserve">Schrag et al. 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__ropinirole_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__placebo_mean-difference</t>
+    <t xml:space="preserve">Spieker et al. 1999</t>
   </si>
   <si>
     <t xml:space="preserve">105</t>
   </si>
   <si>
-    <t xml:space="preserve">Schrag et al. 2002.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__levodopa_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schrag et al. 2002.2</t>
+    <t xml:space="preserve">Su et al. 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items20_21__selegiline-vitaminE_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items20_21__selegiline-vitaminE_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items20_21__placebo-vitaminE_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items20_21__placebo-vitaminE_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">107</t>
   </si>
   <si>
-    <t xml:space="preserve">Sivertsen et al. 1989</t>
-  </si>
-  <si>
-    <t xml:space="preserve">109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spieker et al. 1999</t>
+    <t xml:space="preserve">Tedeschi et al. 1990</t>
   </si>
   <si>
     <t xml:space="preserve">110</t>
   </si>
   <si>
-    <t xml:space="preserve">Su et al. 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_item20_21__placebo-vitaminE_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_item20_21__placebo-vitaminE_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_item20_21__selegiline-vitaminE_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_item20_21__selegiline-vitaminE_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tedeschi et al. 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">115</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vorasoot et al. 2020</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__exercise_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20_21__exercise_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121</t>
+    <t xml:space="preserve">UPDRS_III_items20_21__exercise_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__exercise_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">116</t>
   </si>
   <si>
     <t xml:space="preserve">Zhang et al. 2013</t>
   </si>
   <si>
-    <t xml:space="preserve">122</t>
+    <t xml:space="preserve">117</t>
   </si>
   <si>
     <t xml:space="preserve">Zhang et al. 2018</t>
@@ -641,7 +614,7 @@
     <t xml:space="preserve">UPDRS_III_tremor__control_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">123</t>
+    <t xml:space="preserve">118</t>
   </si>
   <si>
     <t xml:space="preserve">Zhao et al. 2015</t>
@@ -650,22 +623,16 @@
     <t xml:space="preserve">UPDRS_III_item20__droxidopa_baseline</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20__placebo_baseline</t>
-  </si>
-  <si>
     <t xml:space="preserve">UPDRS_III_item20__droxidopa_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20__placebo_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">124</t>
+    <t xml:space="preserve">119</t>
   </si>
   <si>
     <t xml:space="preserve">Zhou et al. 2019</t>
   </si>
   <si>
-    <t xml:space="preserve">125</t>
+    <t xml:space="preserve">120</t>
   </si>
   <si>
     <t xml:space="preserve">Ziegler et al. 2003</t>
@@ -1468,10 +1435,10 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -1482,19 +1449,19 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
         <v>80</v>
       </c>
-      <c r="B21" t="s">
+      <c r="E21" t="s">
         <v>81</v>
-      </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" t="s">
-        <v>41</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
@@ -1505,50 +1472,50 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
         <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G22" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I22" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J22"/>
       <c r="K22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F23"/>
       <c r="G23"/>
@@ -1559,10 +1526,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
@@ -1578,10 +1545,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
@@ -1597,41 +1564,61 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
+      <c r="D26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" t="s">
+        <v>106</v>
+      </c>
+      <c r="I26" t="s">
+        <v>107</v>
+      </c>
+      <c r="J26" t="s">
+        <v>108</v>
+      </c>
+      <c r="K26" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27"/>
-      <c r="G27"/>
+        <v>113</v>
+      </c>
+      <c r="F27" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" t="s">
+        <v>115</v>
+      </c>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -1639,61 +1626,49 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="F28" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="G28" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="H28" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="I28" t="s">
-        <v>111</v>
-      </c>
-      <c r="J28" t="s">
-        <v>112</v>
-      </c>
-      <c r="K28" t="s">
-        <v>113</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="J28"/>
+      <c r="K28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C29" t="s">
         <v>13</v>
       </c>
-      <c r="D29" t="s">
-        <v>116</v>
-      </c>
-      <c r="E29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" t="s">
-        <v>118</v>
-      </c>
-      <c r="G29" t="s">
-        <v>119</v>
-      </c>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -1701,32 +1676,20 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
       </c>
-      <c r="D30" t="s">
-        <v>122</v>
-      </c>
-      <c r="E30" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" t="s">
-        <v>125</v>
-      </c>
-      <c r="H30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30" t="s">
-        <v>23</v>
-      </c>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
     </row>
@@ -1740,10 +1703,18 @@
       <c r="C31" t="s">
         <v>13</v>
       </c>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
+      <c r="D31" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" t="s">
+        <v>131</v>
+      </c>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
@@ -1751,16 +1722,20 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C32" t="s">
         <v>13</v>
       </c>
-      <c r="D32"/>
-      <c r="E32"/>
+      <c r="D32" t="s">
+        <v>134</v>
+      </c>
+      <c r="E32" t="s">
+        <v>135</v>
+      </c>
       <c r="F32"/>
       <c r="G32"/>
       <c r="H32"/>
@@ -1770,19 +1745,19 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C33" t="s">
         <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E33" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F33"/>
       <c r="G33"/>
@@ -1793,20 +1768,16 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
       </c>
-      <c r="D34" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" t="s">
-        <v>133</v>
-      </c>
+      <c r="D34"/>
+      <c r="E34"/>
       <c r="F34"/>
       <c r="G34"/>
       <c r="H34"/>
@@ -1816,10 +1787,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B35" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C35" t="s">
         <v>13</v>
@@ -1835,18 +1806,26 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C36" t="s">
         <v>13</v>
       </c>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
+      <c r="D36" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" t="s">
+        <v>145</v>
+      </c>
+      <c r="F36" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" t="s">
+        <v>115</v>
+      </c>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
@@ -1854,26 +1833,22 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="E37" t="s">
-        <v>143</v>
-      </c>
-      <c r="F37" t="s">
-        <v>118</v>
-      </c>
-      <c r="G37" t="s">
-        <v>119</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F37"/>
+      <c r="G37"/>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
@@ -1881,25 +1856,25 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E38" t="s">
-        <v>27</v>
+        <v>152</v>
       </c>
       <c r="F38" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="G38" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="H38"/>
       <c r="I38"/>
@@ -1908,25 +1883,25 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="E39" t="s">
-        <v>151</v>
+        <v>114</v>
       </c>
       <c r="F39" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G39" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H39"/>
       <c r="I39"/>
@@ -1935,26 +1910,18 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B40" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
       </c>
-      <c r="D40" t="s">
-        <v>116</v>
-      </c>
-      <c r="E40" t="s">
-        <v>118</v>
-      </c>
-      <c r="F40" t="s">
-        <v>117</v>
-      </c>
-      <c r="G40" t="s">
-        <v>119</v>
-      </c>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
@@ -1962,20 +1929,16 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C41" t="s">
         <v>13</v>
       </c>
-      <c r="D41" t="s">
-        <v>156</v>
-      </c>
-      <c r="E41" t="s">
-        <v>157</v>
-      </c>
+      <c r="D41"/>
+      <c r="E41"/>
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41"/>
@@ -1985,18 +1948,26 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C42" t="s">
         <v>13</v>
       </c>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="G42"/>
+      <c r="D42" t="s">
+        <v>161</v>
+      </c>
+      <c r="E42" t="s">
+        <v>162</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" t="s">
+        <v>23</v>
+      </c>
       <c r="H42"/>
       <c r="I42"/>
       <c r="J42"/>
@@ -2004,18 +1975,26 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B43" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
       </c>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="G43"/>
+      <c r="D43" t="s">
+        <v>165</v>
+      </c>
+      <c r="E43" t="s">
+        <v>166</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
       <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
@@ -2023,61 +2002,45 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B44" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E44" t="s">
-        <v>165</v>
-      </c>
-      <c r="F44" t="s">
-        <v>166</v>
-      </c>
-      <c r="G44" t="s">
-        <v>167</v>
-      </c>
-      <c r="H44" t="s">
-        <v>168</v>
-      </c>
-      <c r="I44" t="s">
-        <v>169</v>
-      </c>
-      <c r="J44" t="s">
-        <v>170</v>
-      </c>
-      <c r="K44" t="s">
-        <v>171</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" t="s">
         <v>172</v>
       </c>
-      <c r="B45" t="s">
-        <v>173</v>
-      </c>
-      <c r="C45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" t="s">
-        <v>174</v>
-      </c>
-      <c r="E45" t="s">
-        <v>175</v>
-      </c>
-      <c r="F45" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" t="s">
-        <v>23</v>
-      </c>
+      <c r="F45"/>
+      <c r="G45"/>
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45"/>
@@ -2085,19 +2048,19 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E46" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F46"/>
       <c r="G46"/>
@@ -2108,20 +2071,16 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B47" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
       </c>
-      <c r="D47" t="s">
-        <v>178</v>
-      </c>
-      <c r="E47" t="s">
-        <v>182</v>
-      </c>
+      <c r="D47"/>
+      <c r="E47"/>
       <c r="F47"/>
       <c r="G47"/>
       <c r="H47"/>
@@ -2131,20 +2090,16 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B48" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C48" t="s">
         <v>13</v>
       </c>
-      <c r="D48" t="s">
-        <v>178</v>
-      </c>
-      <c r="E48" t="s">
-        <v>182</v>
-      </c>
+      <c r="D48"/>
+      <c r="E48"/>
       <c r="F48"/>
       <c r="G48"/>
       <c r="H48"/>
@@ -2154,18 +2109,26 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>180</v>
+      </c>
+      <c r="B49" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s">
+        <v>182</v>
+      </c>
+      <c r="E49" t="s">
+        <v>183</v>
+      </c>
+      <c r="F49" t="s">
+        <v>184</v>
+      </c>
+      <c r="G49" t="s">
         <v>185</v>
       </c>
-      <c r="B49" t="s">
-        <v>186</v>
-      </c>
-      <c r="C49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49"/>
-      <c r="E49"/>
-      <c r="F49"/>
-      <c r="G49"/>
       <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
@@ -2173,10 +2136,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" t="s">
         <v>187</v>
-      </c>
-      <c r="B50" t="s">
-        <v>188</v>
       </c>
       <c r="C50" t="s">
         <v>13</v>
@@ -2192,25 +2155,25 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51" t="s">
         <v>189</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
         <v>190</v>
       </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>191</v>
       </c>
-      <c r="E51" t="s">
-        <v>192</v>
-      </c>
       <c r="F51" t="s">
-        <v>193</v>
+        <v>62</v>
       </c>
       <c r="G51" t="s">
-        <v>194</v>
+        <v>63</v>
       </c>
       <c r="H51"/>
       <c r="I51"/>
@@ -2219,18 +2182,26 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B52" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C52" t="s">
         <v>13</v>
       </c>
-      <c r="D52"/>
-      <c r="E52"/>
-      <c r="F52"/>
-      <c r="G52"/>
+      <c r="D52" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" t="s">
+        <v>51</v>
+      </c>
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" t="s">
+        <v>23</v>
+      </c>
       <c r="H52"/>
       <c r="I52"/>
       <c r="J52"/>
@@ -2238,25 +2209,25 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" t="s">
+        <v>195</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" t="s">
+        <v>196</v>
+      </c>
+      <c r="E53" t="s">
         <v>197</v>
       </c>
-      <c r="B53" t="s">
+      <c r="F53" t="s">
         <v>198</v>
       </c>
-      <c r="C53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53" t="s">
-        <v>62</v>
-      </c>
-      <c r="E53" t="s">
-        <v>63</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>199</v>
-      </c>
-      <c r="G53" t="s">
-        <v>200</v>
       </c>
       <c r="H53"/>
       <c r="I53"/>
@@ -2265,25 +2236,25 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>200</v>
+      </c>
+      <c r="B54" t="s">
         <v>201</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
         <v>202</v>
       </c>
-      <c r="C54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" t="s">
-        <v>50</v>
-      </c>
       <c r="E54" t="s">
-        <v>51</v>
+        <v>130</v>
       </c>
       <c r="F54" t="s">
-        <v>22</v>
+        <v>203</v>
       </c>
       <c r="G54" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="H54"/>
       <c r="I54"/>
@@ -2292,26 +2263,18 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B55" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C55" t="s">
         <v>13</v>
       </c>
-      <c r="D55" t="s">
-        <v>205</v>
-      </c>
-      <c r="E55" t="s">
-        <v>206</v>
-      </c>
-      <c r="F55" t="s">
-        <v>207</v>
-      </c>
-      <c r="G55" t="s">
-        <v>208</v>
-      </c>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
       <c r="H55"/>
       <c r="I55"/>
       <c r="J55"/>
@@ -2319,72 +2282,26 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s">
+        <v>208</v>
+      </c>
+      <c r="E56" t="s">
         <v>209</v>
       </c>
-      <c r="B56" t="s">
-        <v>210</v>
-      </c>
-      <c r="C56" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" t="s">
-        <v>211</v>
-      </c>
-      <c r="E56" t="s">
-        <v>212</v>
-      </c>
-      <c r="F56" t="s">
-        <v>213</v>
-      </c>
-      <c r="G56" t="s">
-        <v>214</v>
-      </c>
+      <c r="F56"/>
+      <c r="G56"/>
       <c r="H56"/>
       <c r="I56"/>
       <c r="J56"/>
       <c r="K56"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>215</v>
-      </c>
-      <c r="B57" t="s">
-        <v>216</v>
-      </c>
-      <c r="C57" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
-      <c r="G57"/>
-      <c r="H57"/>
-      <c r="I57"/>
-      <c r="J57"/>
-      <c r="K57"/>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>217</v>
-      </c>
-      <c r="B58" t="s">
-        <v>218</v>
-      </c>
-      <c r="C58" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" t="s">
-        <v>219</v>
-      </c>
-      <c r="E58" t="s">
-        <v>220</v>
-      </c>
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
-      <c r="J58"/>
-      <c r="K58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added further analyses and especially meta-analysis routine
</commit_message>
<xml_diff>
--- a/primary_outcomesRCT.xlsx
+++ b/primary_outcomesRCT.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -62,19 +62,13 @@
     <t xml:space="preserve">UPDRS_III_item20__adenosineA2a_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bergamasco et al. 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
+    <t xml:space="preserve">8</t>
   </si>
   <si>
     <t xml:space="preserve">Bonuccelli et al. 1997</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_item20_22__clozapine_baseline</t>
+    <t xml:space="preserve">UPDRS_III_item20_21__clozapine_baseline</t>
   </si>
   <si>
     <t xml:space="preserve">UPDRS_III_items20_21__clozapine_follow-up</t>
@@ -86,7 +80,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__placebo_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">11</t>
   </si>
   <si>
     <t xml:space="preserve">Cattaneo et al. 2016</t>
@@ -98,39 +92,33 @@
     <t xml:space="preserve">UPDRS_III_items20_21__placebo_mean-difference</t>
   </si>
   <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Craig et al. 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__nmt_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__nmt_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__music-relaxation-control_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__music-relaxation-control_follow-up</t>
+  </si>
+  <si>
     <t xml:space="preserve">15</t>
   </si>
   <si>
-    <t xml:space="preserve">Craig et al. 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__nmt_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__nmt_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__music-relaxation_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__music-relaxation_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
     <t xml:space="preserve">de Faria et al. 2020</t>
   </si>
   <si>
     <t xml:space="preserve">17</t>
   </si>
   <si>
-    <t xml:space="preserve">Eberhardt et al. 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
     <t xml:space="preserve">Elmer (2013)</t>
   </si>
   <si>
@@ -140,7 +128,7 @@
     <t xml:space="preserve">UPDRS_item16_20_21__placebo_adjusted-mean-difference</t>
   </si>
   <si>
-    <t xml:space="preserve">23</t>
+    <t xml:space="preserve">21</t>
   </si>
   <si>
     <t xml:space="preserve">Parkinson Study Group (1999)</t>
@@ -149,7 +137,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__clozapine_mean-difference</t>
   </si>
   <si>
-    <t xml:space="preserve">26</t>
+    <t xml:space="preserve">24</t>
   </si>
   <si>
     <t xml:space="preserve">Goetz et al. 2000</t>
@@ -158,7 +146,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__placebo_percentual-change</t>
   </si>
   <si>
-    <t xml:space="preserve">29</t>
+    <t xml:space="preserve">27</t>
   </si>
   <si>
     <t xml:space="preserve">Hattori et al. 2018</t>
@@ -170,45 +158,45 @@
     <t xml:space="preserve">UPDRS_III_items20_21__rasagiline_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">30</t>
+    <t xml:space="preserve">28</t>
   </si>
   <si>
     <t xml:space="preserve">Heinonen et al. 1989</t>
   </si>
   <si>
-    <t xml:space="preserve">35</t>
+    <t xml:space="preserve">33</t>
   </si>
   <si>
     <t xml:space="preserve">Jankovic et al. 2014</t>
   </si>
   <si>
+    <t xml:space="preserve">37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kadkhodaie et al. 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaut et al. 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__wbv_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__wbv_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__control_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__control_follow-up</t>
+  </si>
+  <si>
     <t xml:space="preserve">39</t>
   </si>
   <si>
-    <t xml:space="preserve">Kadkhodaie et al. 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaut et al. 2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__wbv_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__wbv_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__control_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__control_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41</t>
-  </si>
-  <si>
     <t xml:space="preserve">King et al. 2009</t>
   </si>
   <si>
@@ -218,7 +206,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__vibration_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">45</t>
+    <t xml:space="preserve">43</t>
   </si>
   <si>
     <t xml:space="preserve">Kulisevsky et al. 2002</t>
@@ -230,357 +218,339 @@
     <t xml:space="preserve">UPDRS_III_items20_21__theophylline_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__placebo-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__placebo-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__theophylline-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__theophylline-levodopa_follow-up</t>
+    <t xml:space="preserve">44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laihinen et al. 1992</t>
   </si>
   <si>
     <t xml:space="preserve">46</t>
   </si>
   <si>
-    <t xml:space="preserve">Laihinen et al. 1992</t>
+    <t xml:space="preserve">Lew (2013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__rasagiline_adjusted-mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__placebo_adjusted-mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lew (2013).1</t>
   </si>
   <si>
     <t xml:space="preserve">48</t>
   </si>
   <si>
-    <t xml:space="preserve">Lew (2013)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__rasagiline_adjusted-mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__placebo_adjusted-mean-difference</t>
+    <t xml:space="preserve">Li et al. 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__WG_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__WG_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__TAG_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__TAG_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__SAG-control_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__SAG-control_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">49</t>
   </si>
   <si>
-    <t xml:space="preserve">Lew (2013).1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Li et al. 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__WG_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__WG_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__TAG_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__TAG_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__SAG_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__SAG_follow-up</t>
+    <t xml:space="preserve">Lieberman et al. 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__placebo_percentual_reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__pramipexole_percentual_reduction</t>
   </si>
   <si>
     <t xml:space="preserve">51</t>
   </si>
   <si>
-    <t xml:space="preserve">Lieberman et al. 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__placebo_percentual_reduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__pramipexole_percentual_reduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53</t>
-  </si>
-  <si>
     <t xml:space="preserve">Macht et al. 2000</t>
   </si>
   <si>
-    <t xml:space="preserve">56</t>
+    <t xml:space="preserve">54</t>
   </si>
   <si>
     <t xml:space="preserve">Malsch et al. 2001</t>
   </si>
   <si>
+    <t xml:space="preserve">58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mizuno et al. 1995.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pergolide_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pergolide_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine-levodopa_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine-levodopa_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pergolide-levodopa_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pergolide-levodopa_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moeller et al. 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__pramipexole_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__pramipexole_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__placebo_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__placebo_follow-up</t>
+  </si>
+  <si>
     <t xml:space="preserve">60</t>
   </si>
   <si>
-    <t xml:space="preserve">Mizuno et al. 1995.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__pergolide_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__pergolide_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__pergolide-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__pergolide-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moeller et al. 2005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__pramipexole_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__pramipexole_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__placebo_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__placebo_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62</t>
-  </si>
-  <si>
     <t xml:space="preserve">Montastruc et al. 1999</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__piribedil50_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__piribedil50_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__piribedil100_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__piribedil100_follow-up</t>
+    <t xml:space="preserve">UPDRS_III_item20__piribedil_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__piribedil_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__placebo_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__placebo_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navan et al. 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navan et al. 2003.1</t>
   </si>
   <si>
     <t xml:space="preserve">66</t>
   </si>
   <si>
-    <t xml:space="preserve">Navan et al. 2003</t>
+    <t xml:space="preserve">Nigro et al. 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__apomorphine_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__apomorphine_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">67</t>
   </si>
   <si>
-    <t xml:space="preserve">Navan et al. 2003.1</t>
+    <t xml:space="preserve">Nomoto et al. 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items16_20_21__rotigotine_mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items16_20_21__placebo_mean-difference</t>
   </si>
   <si>
     <t xml:space="preserve">68</t>
   </si>
   <si>
-    <t xml:space="preserve">Nigro et al. 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__apomorphine_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__apomorphine_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__placebo_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__placebo_follow-up</t>
+    <t xml:space="preserve">Nomoto et al. 2018.1</t>
   </si>
   <si>
     <t xml:space="preserve">69</t>
   </si>
   <si>
-    <t xml:space="preserve">Nomoto et al. 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items16_20_21__rotigotine_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items16_20_21__placebo_mean-difference</t>
+    <t xml:space="preserve">Nutt et al. 2007</t>
   </si>
   <si>
     <t xml:space="preserve">70</t>
   </si>
   <si>
-    <t xml:space="preserve">Nomoto et al. 2018.1</t>
+    <t xml:space="preserve">Olanow et al. 1987</t>
   </si>
   <si>
     <t xml:space="preserve">71</t>
   </si>
   <si>
-    <t xml:space="preserve">Nutt et al. 2007</t>
+    <t xml:space="preserve">Olson et al. 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__gabapentin_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__gabapentin_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">72</t>
   </si>
   <si>
-    <t xml:space="preserve">Olanow et al. 1987</t>
+    <t xml:space="preserve">Parkinson Study Group (2007)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__pramipexole_mean-difference</t>
   </si>
   <si>
     <t xml:space="preserve">73</t>
   </si>
   <si>
-    <t xml:space="preserve">Olson et al. 1997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__gabapentin_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__gabapentin_follow-up</t>
+    <t xml:space="preserve">Petramfar et al. 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__licorice_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items16_20_21__licorice_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">74</t>
   </si>
   <si>
-    <t xml:space="preserve">Parkinson Study Group (2007)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__pramipexole_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Petramfar et al. 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__licorice_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items16_20_21__licorice_follow-up</t>
+    <t xml:space="preserve">Pogarell et al. 2002</t>
   </si>
   <si>
     <t xml:space="preserve">76</t>
   </si>
   <si>
-    <t xml:space="preserve">Pogarell et al. 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
     <t xml:space="preserve">Przuntek et al. 2002</t>
   </si>
   <si>
-    <t xml:space="preserve">81</t>
+    <t xml:space="preserve">79</t>
   </si>
   <si>
     <t xml:space="preserve">Rascol et al. 1988</t>
   </si>
   <si>
+    <t xml:space="preserve">93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huebsch et al. 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__qigong_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__qigong_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schneider et al. 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__GM1_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__GM1_follow-up</t>
+  </si>
+  <si>
     <t xml:space="preserve">96</t>
   </si>
   <si>
-    <t xml:space="preserve">Huebsch et al. 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__qigong_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__qigong_follow-up</t>
+    <t xml:space="preserve">Schrag et al. 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__ropinirole_mean-difference</t>
   </si>
   <si>
     <t xml:space="preserve">97</t>
   </si>
   <si>
-    <t xml:space="preserve">Schneider et al. 1998</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__GM1_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__GM1_follow-up</t>
+    <t xml:space="preserve">Schrag et al. 2002.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine_mean-difference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schrag et al. 2002.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_items20_21__levodopa_mean-difference</t>
   </si>
   <si>
     <t xml:space="preserve">99</t>
   </si>
   <si>
-    <t xml:space="preserve">Schrag et al. 2002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__ropinirole_mean-difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schrag et al. 2002.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__bromocriptine_mean-difference</t>
+    <t xml:space="preserve">Sivertsen et al. 1989</t>
   </si>
   <si>
     <t xml:space="preserve">101</t>
   </si>
   <si>
-    <t xml:space="preserve">Schrag et al. 2002.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__levodopa_mean-difference</t>
+    <t xml:space="preserve">Spieker et al. 1999</t>
   </si>
   <si>
     <t xml:space="preserve">102</t>
   </si>
   <si>
-    <t xml:space="preserve">Sivertsen et al. 1989</t>
+    <t xml:space="preserve">Su et al. 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items20_21__selegiline-vitaminE_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items20_21__selegiline-vitaminE_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items20_21__placebo-vitaminE_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_items20_21__placebo-vitaminE_follow-up</t>
   </si>
   <si>
     <t xml:space="preserve">104</t>
   </si>
   <si>
-    <t xml:space="preserve">Spieker et al. 1999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Su et al. 2004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items20_21__selegiline-vitaminE_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items20_21__selegiline-vitaminE_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items20_21__placebo-vitaminE_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_items20_21__placebo-vitaminE_follow-up</t>
+    <t xml:space="preserve">Tedeschi et al. 1990</t>
   </si>
   <si>
     <t xml:space="preserve">107</t>
   </si>
   <si>
-    <t xml:space="preserve">Tedeschi et al. 1990</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110</t>
-  </si>
-  <si>
     <t xml:space="preserve">Vorasoot et al. 2020</t>
   </si>
   <si>
@@ -590,49 +560,49 @@
     <t xml:space="preserve">UPDRS_III_items20_21__exercise_follow-up</t>
   </si>
   <si>
+    <t xml:space="preserve">113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhang et al. 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhang et al. 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_tremor__experimental_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_tremor__control_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_tremor__experimental_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_tremor__control_follow-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhao et al. 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__droxidopa_baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDRS_III_item20__droxidopa_follow-up</t>
+  </si>
+  <si>
     <t xml:space="preserve">116</t>
   </si>
   <si>
-    <t xml:space="preserve">Zhang et al. 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">117</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zhang et al. 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_tremor__experimental_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_tremor__control_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_tremor__experimental_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_tremor__control_follow-up</t>
+    <t xml:space="preserve">Zhou et al. 2019</t>
   </si>
   <si>
     <t xml:space="preserve">118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zhao et al. 2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__droxidopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_item20__droxidopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zhou et al. 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120</t>
   </si>
   <si>
     <t xml:space="preserve">Ziegler et al. 2003</t>
@@ -1041,10 +1011,18 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
       <c r="H3"/>
       <c r="I3"/>
       <c r="J3"/>
@@ -1052,26 +1030,22 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -1079,22 +1053,26 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5"/>
-      <c r="G5"/>
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
       <c r="H5"/>
       <c r="I5"/>
       <c r="J5"/>
@@ -1102,26 +1080,18 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6"/>
@@ -1137,8 +1107,12 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7"/>
-      <c r="E7"/>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7"/>
@@ -1148,16 +1122,20 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
@@ -1167,20 +1145,18 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
       <c r="H9"/>
@@ -1190,22 +1166,26 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10"/>
-      <c r="G10"/>
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
       <c r="H10"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -1213,17 +1193,15 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
+      <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
@@ -1234,26 +1212,22 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F12"/>
+      <c r="G12"/>
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
@@ -1289,13 +1263,17 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14"/>
-      <c r="G14"/>
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
       <c r="H14"/>
       <c r="I14"/>
       <c r="J14"/>
@@ -1303,16 +1281,20 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D15"/>
-      <c r="E15"/>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
       <c r="F15"/>
       <c r="G15"/>
       <c r="H15"/>
@@ -1322,25 +1304,25 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="H16"/>
       <c r="I16"/>
@@ -1349,20 +1331,16 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
-      <c r="D17" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
-      </c>
+      <c r="D17"/>
+      <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
@@ -1372,51 +1350,43 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" t="s">
         <v>73</v>
       </c>
-      <c r="J18" t="s">
-        <v>74</v>
-      </c>
-      <c r="K18" t="s">
-        <v>75</v>
-      </c>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
       </c>
-      <c r="D19"/>
-      <c r="E19"/>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
@@ -1426,42 +1396,50 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
         <v>78</v>
       </c>
-      <c r="B20" t="s">
+      <c r="E20" t="s">
         <v>79</v>
       </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>80</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>81</v>
       </c>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
+      <c r="H20" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" t="s">
+        <v>83</v>
+      </c>
       <c r="J20"/>
       <c r="K20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
@@ -1472,51 +1450,35 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
         <v>13</v>
       </c>
-      <c r="D22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" t="s">
-        <v>90</v>
-      </c>
-      <c r="I22" t="s">
-        <v>91</v>
-      </c>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
       </c>
-      <c r="D23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" t="s">
-        <v>95</v>
-      </c>
+      <c r="D23"/>
+      <c r="E23"/>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
@@ -1526,37 +1488,61 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" t="s">
         <v>96</v>
       </c>
-      <c r="B24" t="s">
+      <c r="G24" t="s">
         <v>97</v>
       </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
+      <c r="H24" t="s">
+        <v>98</v>
+      </c>
+      <c r="I24" t="s">
+        <v>99</v>
+      </c>
+      <c r="J24" t="s">
+        <v>100</v>
+      </c>
+      <c r="K24" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
       </c>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" t="s">
+        <v>107</v>
+      </c>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
@@ -1564,61 +1550,45 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F26" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="G26" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" t="s">
-        <v>106</v>
-      </c>
-      <c r="I26" t="s">
-        <v>107</v>
-      </c>
-      <c r="J26" t="s">
-        <v>108</v>
-      </c>
-      <c r="K26" t="s">
-        <v>109</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" t="s">
-        <v>114</v>
-      </c>
-      <c r="G27" t="s">
-        <v>115</v>
-      </c>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
@@ -1634,41 +1604,37 @@
       <c r="C28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" t="s">
-        <v>119</v>
-      </c>
-      <c r="F28" t="s">
-        <v>120</v>
-      </c>
-      <c r="G28" t="s">
-        <v>121</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" t="s">
-        <v>23</v>
-      </c>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C29" t="s">
         <v>13</v>
       </c>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" t="s">
+        <v>113</v>
+      </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
@@ -1676,16 +1642,20 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
         <v>124</v>
       </c>
-      <c r="B30" t="s">
+      <c r="E30" t="s">
         <v>125</v>
       </c>
-      <c r="C30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30"/>
-      <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30"/>
@@ -1704,17 +1674,13 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E31" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" t="s">
-        <v>130</v>
-      </c>
-      <c r="G31" t="s">
-        <v>131</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
@@ -1722,20 +1688,16 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
         <v>13</v>
       </c>
-      <c r="D32" t="s">
-        <v>134</v>
-      </c>
-      <c r="E32" t="s">
-        <v>135</v>
-      </c>
+      <c r="D32"/>
+      <c r="E32"/>
       <c r="F32"/>
       <c r="G32"/>
       <c r="H32"/>
@@ -1745,20 +1707,16 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
         <v>13</v>
       </c>
-      <c r="D33" t="s">
-        <v>134</v>
-      </c>
-      <c r="E33" t="s">
-        <v>135</v>
-      </c>
+      <c r="D33"/>
+      <c r="E33"/>
       <c r="F33"/>
       <c r="G33"/>
       <c r="H33"/>
@@ -1768,18 +1726,26 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C34" t="s">
         <v>13</v>
       </c>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
+      <c r="D34" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" t="s">
+        <v>135</v>
+      </c>
+      <c r="F34" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" t="s">
+        <v>107</v>
+      </c>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
@@ -1787,16 +1753,20 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C35" t="s">
         <v>13</v>
       </c>
-      <c r="D35"/>
-      <c r="E35"/>
+      <c r="D35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" t="s">
+        <v>25</v>
+      </c>
       <c r="F35"/>
       <c r="G35"/>
       <c r="H35"/>
@@ -1806,25 +1776,25 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" t="s">
         <v>142</v>
       </c>
-      <c r="B36" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" t="s">
-        <v>144</v>
-      </c>
-      <c r="E36" t="s">
-        <v>145</v>
-      </c>
       <c r="F36" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G36" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H36"/>
       <c r="I36"/>
@@ -1833,22 +1803,26 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B37" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s">
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37"/>
-      <c r="G37"/>
+        <v>106</v>
+      </c>
+      <c r="F37" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" t="s">
+        <v>107</v>
+      </c>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
@@ -1856,26 +1830,18 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
       </c>
-      <c r="D38" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" t="s">
-        <v>152</v>
-      </c>
-      <c r="F38" t="s">
-        <v>114</v>
-      </c>
-      <c r="G38" t="s">
-        <v>115</v>
-      </c>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -1883,26 +1849,18 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C39" t="s">
         <v>13</v>
       </c>
-      <c r="D39" t="s">
-        <v>112</v>
-      </c>
-      <c r="E39" t="s">
-        <v>114</v>
-      </c>
-      <c r="F39" t="s">
-        <v>113</v>
-      </c>
-      <c r="G39" t="s">
-        <v>115</v>
-      </c>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -1910,18 +1868,26 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
       </c>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
+      <c r="D40" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" t="s">
+        <v>21</v>
+      </c>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
@@ -1929,18 +1895,26 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C41" t="s">
         <v>13</v>
       </c>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
+      <c r="D41" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" t="s">
+        <v>156</v>
+      </c>
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" t="s">
+        <v>21</v>
+      </c>
       <c r="H41"/>
       <c r="I41"/>
       <c r="J41"/>
@@ -1948,26 +1922,22 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
         <v>159</v>
       </c>
-      <c r="B42" t="s">
-        <v>160</v>
-      </c>
-      <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" t="s">
-        <v>161</v>
-      </c>
       <c r="E42" t="s">
-        <v>162</v>
-      </c>
-      <c r="F42" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" t="s">
-        <v>23</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F42"/>
+      <c r="G42"/>
       <c r="H42"/>
       <c r="I42"/>
       <c r="J42"/>
@@ -1975,26 +1945,22 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B43" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E43" t="s">
-        <v>166</v>
-      </c>
-      <c r="F43" t="s">
-        <v>22</v>
-      </c>
-      <c r="G43" t="s">
-        <v>23</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="F43"/>
+      <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
@@ -2002,19 +1968,19 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B44" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E44" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="F44"/>
       <c r="G44"/>
@@ -2025,20 +1991,16 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C45" t="s">
         <v>13</v>
       </c>
-      <c r="D45" t="s">
-        <v>169</v>
-      </c>
-      <c r="E45" t="s">
-        <v>172</v>
-      </c>
+      <c r="D45"/>
+      <c r="E45"/>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45"/>
@@ -2048,20 +2010,16 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B46" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
       </c>
-      <c r="D46" t="s">
-        <v>169</v>
-      </c>
-      <c r="E46" t="s">
-        <v>175</v>
-      </c>
+      <c r="D46"/>
+      <c r="E46"/>
       <c r="F46"/>
       <c r="G46"/>
       <c r="H46"/>
@@ -2071,18 +2029,26 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
       </c>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-      <c r="G47"/>
+      <c r="D47" t="s">
+        <v>172</v>
+      </c>
+      <c r="E47" t="s">
+        <v>173</v>
+      </c>
+      <c r="F47" t="s">
+        <v>174</v>
+      </c>
+      <c r="G47" t="s">
+        <v>175</v>
+      </c>
       <c r="H47"/>
       <c r="I47"/>
       <c r="J47"/>
@@ -2090,10 +2056,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B48" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C48" t="s">
         <v>13</v>
@@ -2109,25 +2075,25 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s">
         <v>180</v>
       </c>
-      <c r="B49" t="s">
+      <c r="E49" t="s">
         <v>181</v>
       </c>
-      <c r="C49" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" t="s">
-        <v>182</v>
-      </c>
-      <c r="E49" t="s">
-        <v>183</v>
-      </c>
       <c r="F49" t="s">
-        <v>184</v>
+        <v>58</v>
       </c>
       <c r="G49" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
       <c r="H49"/>
       <c r="I49"/>
@@ -2136,18 +2102,26 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C50" t="s">
         <v>13</v>
       </c>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
-      <c r="G50"/>
+      <c r="D50" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" t="s">
+        <v>47</v>
+      </c>
+      <c r="F50" t="s">
+        <v>20</v>
+      </c>
+      <c r="G50" t="s">
+        <v>21</v>
+      </c>
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>
@@ -2155,25 +2129,25 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>186</v>
+      </c>
+      <c r="E51" t="s">
+        <v>187</v>
+      </c>
+      <c r="F51" t="s">
         <v>188</v>
       </c>
-      <c r="B51" t="s">
+      <c r="G51" t="s">
         <v>189</v>
-      </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
-        <v>190</v>
-      </c>
-      <c r="E51" t="s">
-        <v>191</v>
-      </c>
-      <c r="F51" t="s">
-        <v>62</v>
-      </c>
-      <c r="G51" t="s">
-        <v>63</v>
       </c>
       <c r="H51"/>
       <c r="I51"/>
@@ -2182,25 +2156,25 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
         <v>192</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" t="s">
+        <v>112</v>
+      </c>
+      <c r="F52" t="s">
         <v>193</v>
       </c>
-      <c r="C52" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" t="s">
-        <v>51</v>
-      </c>
-      <c r="F52" t="s">
-        <v>22</v>
-      </c>
       <c r="G52" t="s">
-        <v>23</v>
+        <v>113</v>
       </c>
       <c r="H52"/>
       <c r="I52"/>
@@ -2217,18 +2191,10 @@
       <c r="C53" t="s">
         <v>13</v>
       </c>
-      <c r="D53" t="s">
-        <v>196</v>
-      </c>
-      <c r="E53" t="s">
-        <v>197</v>
-      </c>
-      <c r="F53" t="s">
-        <v>198</v>
-      </c>
-      <c r="G53" t="s">
-        <v>199</v>
-      </c>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
       <c r="H53"/>
       <c r="I53"/>
       <c r="J53"/>
@@ -2236,72 +2202,26 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B54" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C54" t="s">
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E54" t="s">
-        <v>130</v>
-      </c>
-      <c r="F54" t="s">
-        <v>203</v>
-      </c>
-      <c r="G54" t="s">
-        <v>131</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="F54"/>
+      <c r="G54"/>
       <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
       <c r="K54"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>204</v>
-      </c>
-      <c r="B55" t="s">
-        <v>205</v>
-      </c>
-      <c r="C55" t="s">
-        <v>13</v>
-      </c>
-      <c r="D55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-      <c r="I55"/>
-      <c r="J55"/>
-      <c r="K55"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>206</v>
-      </c>
-      <c r="B56" t="s">
-        <v>207</v>
-      </c>
-      <c r="C56" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" t="s">
-        <v>208</v>
-      </c>
-      <c r="E56" t="s">
-        <v>209</v>
-      </c>
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-      <c r="I56"/>
-      <c r="J56"/>
-      <c r="K56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>